<commit_message>
Changed Quantity and randomized invoice number
</commit_message>
<xml_diff>
--- a/Output_Data/output_Data_00000015.xlsx
+++ b/Output_Data/output_Data_00000015.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adithya\Documents\UiPath\Task\Output_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A2D8EF-A1F7-4A33-90CA-9BA52D1B333C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB8E6D1-465D-438C-9359-520BA26742EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="2350" windowWidth="6410" windowHeight="3270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7900" yWindow="5750" windowWidth="6410" windowHeight="3270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>INVOICE</t>
   </si>
@@ -69,13 +69,41 @@
     <t>Rate /Hour</t>
   </si>
   <si>
-    <t>Overhead Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spare Parts </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Labour Cost </t>
+    <t>(Company Name)</t>
+  </si>
+  <si>
+    <t>1-2019-20727</t>
+  </si>
+  <si>
+    <t>2009-TOYOTA-PRADO</t>
+  </si>
+  <si>
+    <t>A40511</t>
+  </si>
+  <si>
+    <t>08889-80039-0 N/A; COOLANT LONG LIFE 1L 16400-31354-0</t>
+  </si>
+  <si>
+    <t>N/A; RADIATOR ASSY 16571-31130-0</t>
+  </si>
+  <si>
+    <t>N/A; HOSE- RADIATOR- 16572-31170-0</t>
+  </si>
+  <si>
+    <t>N/A; HOSE- RADIATOR-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Labour
+</t>
+  </si>
+  <si>
+    <t>Spare Parts</t>
+  </si>
+  <si>
+    <t>Labour Cost</t>
+  </si>
+  <si>
+    <t>Overhead Costs</t>
   </si>
   <si>
     <t>Total Cost</t>
@@ -85,27 +113,6 @@
   </si>
   <si>
     <t>GRAND TOTAL</t>
-  </si>
-  <si>
-    <t>(Company Name)</t>
-  </si>
-  <si>
-    <t>1-2019-20727</t>
-  </si>
-  <si>
-    <t>2009-TOYOTA-PRADO</t>
-  </si>
-  <si>
-    <t>08889-80039-0 N/A; COOLANT LONG LIFE 1L 16400-31354-0</t>
-  </si>
-  <si>
-    <t>N/A; RADIATOR ASSY 16571-31130-0</t>
-  </si>
-  <si>
-    <t>N/A; HOSE- RADIATOR- 16572-31170-0</t>
-  </si>
-  <si>
-    <t>N/A; HOSE- RADIATOR-</t>
   </si>
 </sst>
 </file>
@@ -155,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -179,26 +186,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -282,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -290,22 +277,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -606,19 +594,19 @@
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.5">
       <c r="B2" s="5"/>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
       <c r="G2" s="6"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="7"/>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -652,8 +640,8 @@
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
-        <v>100478600800003</v>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -665,7 +653,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -677,7 +665,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -727,33 +715,25 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="7"/>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="4">
-        <v>22</v>
-      </c>
-      <c r="F13" s="4">
-        <v>88</v>
-      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="7"/>
       <c r="C14" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="18">
-        <v>1359.05</v>
-      </c>
-      <c r="F14" s="18">
-        <v>1359.05</v>
+        <v>18</v>
+      </c>
+      <c r="E14" s="4">
+        <v>22</v>
+      </c>
+      <c r="F14" s="4">
+        <v>88</v>
       </c>
       <c r="G14" s="8"/>
     </row>
@@ -763,13 +743,13 @@
         <v>1</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="4">
-        <v>31.19</v>
-      </c>
-      <c r="F15" s="4">
-        <v>31.19</v>
+        <v>19</v>
+      </c>
+      <c r="E15" s="14">
+        <v>1359.05</v>
+      </c>
+      <c r="F15" s="14">
+        <v>1359.05</v>
       </c>
       <c r="G15" s="8"/>
     </row>
@@ -779,22 +759,30 @@
         <v>1</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="4">
-        <v>31.57</v>
-      </c>
-      <c r="F16" s="4">
-        <v>31.57</v>
+        <v>20</v>
+      </c>
+      <c r="E16" s="14">
+        <v>31.19</v>
+      </c>
+      <c r="F16" s="14">
+        <v>31.19</v>
       </c>
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B17" s="7"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="14">
+        <v>31.57</v>
+      </c>
+      <c r="F17" s="14">
+        <v>31.57</v>
+      </c>
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
@@ -807,17 +795,15 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" s="7"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B20" s="7"/>
-      <c r="C20" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -825,62 +811,68 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B21" s="7"/>
-      <c r="C21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
       <c r="G21" s="8"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" s="7"/>
-      <c r="C22" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4">
-        <v>150.04</v>
-      </c>
-      <c r="F22" s="4">
-        <v>37.51</v>
+      <c r="C22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B23" s="7"/>
-      <c r="C23" s="4">
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B24" s="7"/>
+      <c r="C24" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="4">
+        <v>150.04</v>
+      </c>
+      <c r="F24" s="4">
+        <v>37.51</v>
+      </c>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="7"/>
+      <c r="C25" s="4">
         <v>2</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4">
+      <c r="D25" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="4">
         <v>150</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F25" s="4">
         <v>300</v>
       </c>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B24" s="7"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B25" s="7"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
       <c r="G25" s="8"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.35">
@@ -912,9 +904,9 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="14">
+        <v>23</v>
+      </c>
+      <c r="F29" s="17">
         <v>1509.81</v>
       </c>
       <c r="G29" s="8"/>
@@ -924,7 +916,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F30" s="2">
         <v>337.51</v>
@@ -936,7 +928,7 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F31" s="2">
         <v>0</v>
@@ -948,9 +940,9 @@
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" s="15">
+        <v>26</v>
+      </c>
+      <c r="F32" s="17">
         <v>1847.31</v>
       </c>
       <c r="G32" s="8"/>
@@ -960,26 +952,26 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F33" s="2">
         <v>92.37</v>
       </c>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B34" s="7"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="16">
+        <v>28</v>
+      </c>
+      <c r="F34" s="17">
         <v>1939.68</v>
       </c>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>

</xml_diff>